<commit_message>
Mundanças Gerais: Em models, trabalhei nas functions e importei elas no tests para avaliar cada cenário do anki
</commit_message>
<xml_diff>
--- a/Data/cards.xlsx
+++ b/Data/cards.xlsx
@@ -61,21 +61,6 @@
     <t>Quais palavras-chave normalmente indicam “informações certas” e quais indicam “informações inferidas” num enunciado de questão?</t>
   </si>
   <si>
-    <r>
-      <t>Informação Certa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (compreensão): “afirma”, “diz”, “relata”, “mostra”, “evidencia”, “de acordo com o texto” etc.</t>
-    </r>
-  </si>
-  <si>
     <t>Cartão 5</t>
   </si>
   <si>
@@ -92,13 +77,16 @@
   </si>
   <si>
     <t>Na tirinha do Armandinho (exemplo IFRR/2020), conclui-se que “punir é mais fácil que educar”, mas não necessariamente mais eficiente. Essa “eficiência” surge como inferência lógica (interpretação), enquanto a facilidade de punir está subentendida como pressuposto (compreensão).</t>
+  </si>
+  <si>
+    <t>Informação Certa (compreensão): “afirma”, “diz”, “relata”, “mostra”, “evidencia”, “de acordo com o texto” etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,23 +95,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -150,22 +122,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,92 +438,92 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="27.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Programa redondo e funcional
</commit_message>
<xml_diff>
--- a/Data/cards.xlsx
+++ b/Data/cards.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Cartão 1</t>
-  </si>
-  <si>
-    <t>O que é compreensão textual?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Front</t>
   </si>
@@ -33,60 +27,449 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>É a identificação direta de informações expressas ou pressupostas no texto, levando a uma certeza. Baseia-se em elementos que estão claramente no texto ou podem ser deduzidos por aspectos gramaticais ou lógicos.</t>
-  </si>
-  <si>
-    <t>Cartão 2</t>
-  </si>
-  <si>
-    <t>O que é interpretação textual?</t>
-  </si>
-  <si>
-    <t>É a inferência de possíveis sentidos, a partir de pistas do texto e do conhecimento de mundo do leitor. Envolve hipóteses e pode não ter uma única resposta exata.</t>
-  </si>
-  <si>
-    <t>Cartão 3</t>
-  </si>
-  <si>
-    <t>Qual a diferença básica entre compreensão e interpretação?</t>
-  </si>
-  <si>
-    <t>Compreensão: foca em informações explícitas ou pressupostas, fornecendo certeza.
-Interpretação: foca em possibilidades e inferências, que dependem de confirmação ou leitura subjetiva.</t>
-  </si>
-  <si>
-    <t>Cartão 4</t>
-  </si>
-  <si>
-    <t>Quais palavras-chave normalmente indicam “informações certas” e quais indicam “informações inferidas” num enunciado de questão?</t>
-  </si>
-  <si>
-    <t>Cartão 5</t>
-  </si>
-  <si>
-    <t>Como o uso do artigo definido (por exemplo, “do”, “da”) pode indicar um pressuposto no texto?</t>
-  </si>
-  <si>
-    <t>O artigo definido indica que algo é apresentado como já conhecido ou reconhecível. Exemplo: “do projeto civilizador” pressupõe que o leitor já tenha ouvido falar do tal projeto.</t>
-  </si>
-  <si>
-    <t>Cartão 6</t>
-  </si>
-  <si>
-    <t>Dê um exemplo prático em que a escolha de punir ou educar foi interpretada no texto de forma a demonstrar pressupostos e inferências.</t>
-  </si>
-  <si>
-    <t>Na tirinha do Armandinho (exemplo IFRR/2020), conclui-se que “punir é mais fácil que educar”, mas não necessariamente mais eficiente. Essa “eficiência” surge como inferência lógica (interpretação), enquanto a facilidade de punir está subentendida como pressuposto (compreensão).</t>
-  </si>
-  <si>
-    <t>Informação Certa (compreensão): “afirma”, “diz”, “relata”, “mostra”, “evidencia”, “de acordo com o texto” etc.</t>
+    <r>
+      <t>Card 31 (Data Science)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Defina overfitting.</t>
+    </r>
+  </si>
+  <si>
+    <t>Quando o modelo ML se ajusta demais ao conjunto de treino, prejudicando a generalização em dados novos.</t>
+  </si>
+  <si>
+    <t>DataScience Overfitting</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 32 (Data Science)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – O que é batch size?</t>
+    </r>
+  </si>
+  <si>
+    <t>Tamanho do “lote” de exemplos processados em cada iteração de treinamento de rede neural.</t>
+  </si>
+  <si>
+    <t>DataScience ML</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 33 (BancoDados)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – O que é uma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>foreign key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?</t>
+    </r>
+  </si>
+  <si>
+    <t>É a chave que referencia outra tabela para criar relacionamento e integridade referencial.</t>
+  </si>
+  <si>
+    <t>BancoDados FK</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 34 (BancoDados)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – DDL vs. DML?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DDL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Data Definition Language) cria ou altera estrutura de objetos (CREATE, DROP), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DML</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Data Manipulation Language) insere ou consulta dados (INSERT, SELECT).</t>
+    </r>
+  </si>
+  <si>
+    <t>BancoDados SQL</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 35 (EngSoft)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – RAD?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rapid Application Development</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; metodologia de desenvolvimento rápido, com prototipagem e feedback contínuo.</t>
+    </r>
+  </si>
+  <si>
+    <t>EngSoft Metodologia</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 36 (EngSoft)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Defina UML Use Case.</t>
+    </r>
+  </si>
+  <si>
+    <t>Diagrama que descreve interações entre atores e o sistema, representando funcionalidades de alto nível.</t>
+  </si>
+  <si>
+    <t>EngSoft UML</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 37 (Infra)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – O que é VLAN?</t>
+    </r>
+  </si>
+  <si>
+    <t>Redes locais virtuais que segmentam logicamente a rede, mesmo usando infraestrutura física compartilhada.</t>
+  </si>
+  <si>
+    <t>Infra Redes</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 38 (Infra)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – SMTP?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Simple Mail Transfer Protocol</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – protocolo de envio/roteamento de emails na camada de aplicação.</t>
+    </r>
+  </si>
+  <si>
+    <t>Infra Redes SMTP</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 39 (Segurança)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – VPN?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Virtual Private Network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – cria um túnel criptografado para comunicação segura entre redes/hosts remotos.</t>
+    </r>
+  </si>
+  <si>
+    <t>Seguranca Infra</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 40 (Segurança)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Keylogger?</t>
+    </r>
+  </si>
+  <si>
+    <t>Malware ou dispositivo que capta as teclas digitadas, podendo roubar senhas e dados sensíveis.</t>
+  </si>
+  <si>
+    <t>Seguranca Malware</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 41 (GestaoTI)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Kanban?</t>
+    </r>
+  </si>
+  <si>
+    <t>Método de trabalho ágil que visualiza fluxo de tarefas em quadros, limitando trabalho em andamento (WIP).</t>
+  </si>
+  <si>
+    <t>GestaoTI Agile</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 42 (GestaoTI)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Escopo em PMBOK?</t>
+    </r>
+  </si>
+  <si>
+    <t>Define os limites e entregas do projeto, evitando funções extras sem aprovação (scope creep).</t>
+  </si>
+  <si>
+    <t>GestaoTI PMBOK</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 43 (Concurso)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Nota de corte?</t>
+    </r>
+  </si>
+  <si>
+    <t>Pontuação mínima para ficar entre os classificados. Varia conforme desempenho geral dos candidatos.</t>
+  </si>
+  <si>
+    <t>Concurso Conceito</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 44 (Lógica)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Negação de (P e Q)?</t>
+    </r>
+  </si>
+  <si>
+    <t>É (¬P) ou (¬Q). Pela lei de De Morgan, nega-se cada proposição e troca-se “e” por “ou”.</t>
+  </si>
+  <si>
+    <t>Logica DeMorgan</t>
+  </si>
+  <si>
+    <r>
+      <t>Card 45 (Estatística)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Qual a diferença entre moda e mediana?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Moda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é o valor mais frequente, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mediana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é o valor central em dados ordenados.</t>
+    </r>
+  </si>
+  <si>
+    <t>Estatistica Medidas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +483,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +524,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,96 +834,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>